<commit_message>
Add Final Project Deliverables directory with all required deliverables
</commit_message>
<xml_diff>
--- a/exports/Candelaria_Inference.xlsx
+++ b/exports/Candelaria_Inference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanj\Desktop\Elective 4\exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Elective 4\Elective 4_3DEFV\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B75818A-1CA6-4754-9B41-013A6CBCEE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239945A9-AF5C-4237-9634-A73FD9950D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inference" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>